<commit_message>
Update reusable methods addition
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata/testdata.xlsx
+++ b/src/test/resources/testdata/testdata.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gopinath\IdeaProjects\Symex\src\test\resources\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44B7A6E4-9331-489A-9147-5D3CF8F065F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A88F49B8-DC79-4DDF-B754-318EF886DCA9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="855" yWindow="3075" windowWidth="23145" windowHeight="6765" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2340" yWindow="2340" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="12">
   <si>
     <t>titleValidationTest</t>
   </si>
@@ -48,23 +48,26 @@
     <t>Dummy</t>
   </si>
   <si>
-    <t>Symx@15#</t>
-  </si>
-  <si>
     <t>expectedTitle</t>
   </si>
   <si>
     <t>Symex</t>
   </si>
   <si>
-    <t>Gopinath</t>
+    <t>System</t>
+  </si>
+  <si>
+    <t>Symx@4321</t>
+  </si>
+  <si>
+    <t>Symx@4322</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -76,6 +79,12 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -388,14 +397,14 @@
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="23.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="13.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -410,7 +419,7 @@
         <v>3</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -418,13 +427,13 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C2" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>9</v>
+      <c r="D2" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -432,13 +441,13 @@
         <v>4</v>
       </c>
       <c r="B3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>9</v>
+        <v>11</v>
+      </c>
+      <c r="D3" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -456,6 +465,7 @@
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>